<commit_message>
Add login and logut for user authentication
</commit_message>
<xml_diff>
--- a/expenditure.xlsx
+++ b/expenditure.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,17 +463,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2024-04-16</t>
+          <t>2024-04-07</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Breakfast</t>
+          <t>Dinner</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>560</t>
+          <t>235</t>
         </is>
       </c>
     </row>
@@ -485,29 +485,29 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2024-04-15</t>
+          <t>2024-04-09</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Dinner</t>
+          <t>Breakfast</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>450</t>
+          <t>340</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Ram Chaudhary</t>
+          <t>Asmin Dhakal</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2024-04-10</t>
+          <t>2024-04-01</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -517,7 +517,51 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>230</t>
+          <t>5000</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>2024-03-31</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Breakfast</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>245</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Asmin Dhakal</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>2024-04-08</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Breakfast</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>200</t>
         </is>
       </c>
     </row>

</xml_diff>